<commit_message>
FUNCTIONALITY: AllowImportPermissions - Updated a test cases. Tabs - Wrote a new suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/Installation/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/Installation/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Title</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t>DefaultObjects</t>
+  </si>
+  <si>
+    <t>Tabs</t>
+  </si>
+  <si>
+    <t>Suited To Manual</t>
+  </si>
+  <si>
+    <t>Application Installation/Upgrading</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -147,7 +162,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -534,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -565,7 +647,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) -1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -584,16 +666,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -604,17 +686,43 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="5"/>
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -632,7 +740,7 @@
       </c>
       <c r="G6" s="9">
         <f>G5/G4</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -650,34 +758,34 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D1 D4:D1048576">
-    <cfRule type="containsText" dxfId="8" priority="14" operator="containsText" text="Outdated">
+  <conditionalFormatting sqref="D1 D5:D1048576">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Outdated">
       <formula>NOT(ISERROR(SEARCH("Outdated",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3">
-    <cfRule type="containsText" dxfId="7" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D2:D4">
+    <cfRule type="containsText" dxfId="15" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="14" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="13" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="12" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="11" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="10" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="9" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
+    <cfRule type="containsText" dxfId="8" priority="8" stopIfTrue="1" operator="containsText" text="Suited to Manual">
       <formula>NOT(ISERROR(SEARCH("Suited to Manual",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>